<commit_message>
Made the ControlUnit class
</commit_message>
<xml_diff>
--- a/documentation/microinstructions.xlsx
+++ b/documentation/microinstructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwa\IdeaProjects\CPUEmulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF77630-B80C-4EDF-824D-64861D4A4B95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB634E8-96F6-4DAE-8A7D-C746AB5B807F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>ALUOpcode</t>
   </si>
   <si>
-    <t>Zout</t>
-  </si>
-  <si>
     <t>PCIn</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>R1 &lt;- R1 + R2</t>
+  </si>
+  <si>
+    <t>ZOut</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T31" sqref="T31"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -490,42 +490,42 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
       <c r="T1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2"/>
     </row>
@@ -593,7 +593,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2"/>
     </row>
@@ -661,7 +661,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -729,7 +729,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2"/>
     </row>
@@ -797,7 +797,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2"/>
     </row>
@@ -865,7 +865,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -933,7 +933,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2"/>
     </row>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2"/>
       <c r="H16" s="1"/>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2"/>
       <c r="H18" s="1"/>
@@ -1302,15 +1302,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added tests and javadoc for the ControlUnit
</commit_message>
<xml_diff>
--- a/documentation/microinstructions.xlsx
+++ b/documentation/microinstructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwa\IdeaProjects\CPUEmulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB634E8-96F6-4DAE-8A7D-C746AB5B807F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81077F05-8F00-4C74-BEA4-5FD1BFD5F592}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>RFIn</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>ZOut</t>
+  </si>
+  <si>
+    <t>R1 &lt;- INTER</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,7 +940,7 @@
       </c>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1070,29 +1073,29 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1134,89 +1137,34 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1228,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1262,10 +1210,128 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H22" s="1"/>
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="H23" s="1"/>
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
@@ -1300,17 +1366,24 @@
     <row r="34" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H34" s="1"/>
     </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a simple test for the ControlUnit
</commit_message>
<xml_diff>
--- a/documentation/microinstructions.xlsx
+++ b/documentation/microinstructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwa\IdeaProjects\CPUEmulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81077F05-8F00-4C74-BEA4-5FD1BFD5F592}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0800CC-1200-40AE-9B70-B8DB1DFC3F89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -445,7 +445,7 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -644,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
         <v>0</v>

</xml_diff>

<commit_message>
Added the circuitry for the ALU
</commit_message>
<xml_diff>
--- a/documentation/microinstructions.xlsx
+++ b/documentation/microinstructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwa\IdeaProjects\CPUEmulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0800CC-1200-40AE-9B70-B8DB1DFC3F89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A43FF0B-25FD-492E-96FD-B1ED8FEE16AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>RFIn</t>
   </si>
@@ -121,6 +121,27 @@
   </si>
   <si>
     <t>R1 &lt;- INTER</t>
+  </si>
+  <si>
+    <t>isJump</t>
+  </si>
+  <si>
+    <t>jmpInterest</t>
+  </si>
+  <si>
+    <t>jmpCond</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>clrFlags</t>
+  </si>
+  <si>
+    <t>setFlag</t>
+  </si>
+  <si>
+    <t>1111</t>
   </si>
 </sst>
 </file>
@@ -442,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,9 +483,10 @@
     <col min="17" max="17" width="15.85546875" customWidth="1"/>
     <col min="18" max="18" width="12" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -525,14 +547,30 @@
       <c r="T1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" t="s">
+        <v>33</v>
+      </c>
+      <c r="W1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -593,14 +631,32 @@
       <c r="T3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -661,14 +717,32 @@
       <c r="T5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="Y6" s="1"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -729,14 +803,32 @@
       <c r="T7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -797,14 +889,32 @@
       <c r="T9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="Y10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -865,14 +975,32 @@
       <c r="T11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -933,14 +1061,32 @@
       <c r="T13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="Y14" s="1"/>
+    </row>
+    <row r="15" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -1001,15 +1147,33 @@
       <c r="T15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="2"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="Y16" s="1"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1070,15 +1234,33 @@
       <c r="T17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="2"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1139,15 +1321,33 @@
       <c r="T19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="2"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1208,8 +1408,23 @@
       <c r="T21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1270,8 +1485,23 @@
       <c r="T22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1332,45 +1562,111 @@
       <c r="T23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="Y25" s="1"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="Y26" s="1"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="Y27" s="1"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="Y29" s="1"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="Y30" s="1"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="Y31" s="1"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="Y32" s="1"/>
+    </row>
+    <row r="33" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="Y33" s="1"/>
+    </row>
+    <row r="34" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="Y34" s="1"/>
+    </row>
+    <row r="35" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="Y35" s="1"/>
+    </row>
+    <row r="36" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="Y36" s="1"/>
+    </row>
+    <row r="37" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="W37" s="1"/>
+      <c r="Y37" s="1"/>
+    </row>
+    <row r="38" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="Y38" s="1"/>
+    </row>
+    <row r="39" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="Y39" s="1"/>
+    </row>
+    <row r="40" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="Y40" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Added jump logic for the microprocessor
</commit_message>
<xml_diff>
--- a/documentation/microinstructions.xlsx
+++ b/documentation/microinstructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwa\IdeaProjects\CPUEmulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A43FF0B-25FD-492E-96FD-B1ED8FEE16AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAA8674-94E5-44DA-91F4-3E7D09BB47AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added unconditional jump check and instruction
</commit_message>
<xml_diff>
--- a/documentation/microinstructions.xlsx
+++ b/documentation/microinstructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwa\IdeaProjects\CPUEmulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAA8674-94E5-44DA-91F4-3E7D09BB47AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9753F1D9-92EC-4895-93E4-2226D17BE73E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
   <si>
     <t>RFIn</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>1111</t>
+  </si>
+  <si>
+    <t>JUMP INTER</t>
   </si>
 </sst>
 </file>
@@ -465,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,28 +1582,245 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2"/>
       <c r="H24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="Y24" s="1"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="H25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="Y25" s="1"/>
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="H26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="Y26" s="1"/>
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="H27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="Y27" s="1"/>
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>1</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
@@ -1669,7 +1889,8 @@
       <c r="Y40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>

</xml_diff>

<commit_message>
Added tests for the CPU instructions
</commit_message>
<xml_diff>
--- a/documentation/microinstructions.xlsx
+++ b/documentation/microinstructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janwa\IdeaProjects\CPUEmulator\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBBE7E4-38E0-43D2-9B25-F31F908711D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AEA7FA-22EF-4CD9-AAE6-42F1F10D74FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,9 +250,6 @@
     <t>R2 &lt;- R2 + 1</t>
   </si>
   <si>
-    <t>R2 &lt;- R1 -  R2</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>94</t>
+  </si>
+  <si>
+    <t>R2 &lt;- R1 - R2</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4207,14 +4207,14 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -4338,7 +4338,7 @@
         <v>0</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I53" s="5">
         <v>1</v>
@@ -4471,14 +4471,14 @@
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
@@ -4602,7 +4602,7 @@
         <v>0</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I57" s="5">
         <v>1</v>
@@ -4735,14 +4735,14 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -4866,7 +4866,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I61" s="5">
         <v>1</v>
@@ -4999,14 +4999,14 @@
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -5053,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I64" s="5">
         <v>1</v>
@@ -5186,14 +5186,14 @@
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -5240,58 +5240,58 @@
         <v>0</v>
       </c>
       <c r="H67" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I67" s="5">
+        <v>1</v>
+      </c>
+      <c r="J67" s="5">
+        <v>0</v>
+      </c>
+      <c r="K67" s="5">
+        <v>0</v>
+      </c>
+      <c r="L67" s="5">
+        <v>0</v>
+      </c>
+      <c r="M67" s="5">
+        <v>0</v>
+      </c>
+      <c r="N67" s="5">
+        <v>0</v>
+      </c>
+      <c r="O67" s="5">
+        <v>0</v>
+      </c>
+      <c r="P67" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="5">
+        <v>0</v>
+      </c>
+      <c r="R67" s="5">
+        <v>0</v>
+      </c>
+      <c r="S67" s="5">
+        <v>0</v>
+      </c>
+      <c r="T67" s="5">
+        <v>0</v>
+      </c>
+      <c r="U67" s="5">
+        <v>0</v>
+      </c>
+      <c r="V67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W67" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X67" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="I67" s="5">
-        <v>1</v>
-      </c>
-      <c r="J67" s="5">
-        <v>0</v>
-      </c>
-      <c r="K67" s="5">
-        <v>0</v>
-      </c>
-      <c r="L67" s="5">
-        <v>0</v>
-      </c>
-      <c r="M67" s="5">
-        <v>0</v>
-      </c>
-      <c r="N67" s="5">
-        <v>0</v>
-      </c>
-      <c r="O67" s="5">
-        <v>0</v>
-      </c>
-      <c r="P67" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="5">
-        <v>0</v>
-      </c>
-      <c r="R67" s="5">
-        <v>0</v>
-      </c>
-      <c r="S67" s="5">
-        <v>0</v>
-      </c>
-      <c r="T67" s="5">
-        <v>0</v>
-      </c>
-      <c r="U67" s="5">
-        <v>0</v>
-      </c>
-      <c r="V67" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W67" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="X67" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y67" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
@@ -5373,14 +5373,14 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -5504,7 +5504,7 @@
         <v>0</v>
       </c>
       <c r="H71" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I71" s="5">
         <v>1</v>
@@ -5555,7 +5555,7 @@
         <v>0</v>
       </c>
       <c r="Y71" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:25" x14ac:dyDescent="0.25">
@@ -5637,14 +5637,14 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D73" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
@@ -5768,7 +5768,7 @@
         <v>0</v>
       </c>
       <c r="H75" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I75" s="5">
         <v>1</v>
@@ -5819,7 +5819,7 @@
         <v>0</v>
       </c>
       <c r="Y75" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.25">
@@ -5901,14 +5901,14 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
@@ -6032,7 +6032,7 @@
         <v>0</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I79" s="5">
         <v>1</v>
@@ -6083,7 +6083,7 @@
         <v>0</v>
       </c>
       <c r="Y79" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
@@ -6165,14 +6165,14 @@
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
@@ -6296,7 +6296,7 @@
         <v>0</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I83" s="5">
         <v>1</v>
@@ -6347,7 +6347,7 @@
         <v>0</v>
       </c>
       <c r="Y83" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:25" x14ac:dyDescent="0.25">
@@ -6429,14 +6429,14 @@
     </row>
     <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -6560,7 +6560,7 @@
         <v>0</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I87" s="5">
         <v>1</v>
@@ -6611,7 +6611,7 @@
         <v>0</v>
       </c>
       <c r="Y87" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="88" spans="1:25" x14ac:dyDescent="0.25">
@@ -6693,14 +6693,14 @@
     </row>
     <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D89" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -6824,7 +6824,7 @@
         <v>0</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I91" s="5">
         <v>1</v>
@@ -6875,7 +6875,7 @@
         <v>0</v>
       </c>
       <c r="Y91" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
@@ -6957,14 +6957,14 @@
     </row>
     <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -7088,7 +7088,7 @@
         <v>0</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I95" s="5">
         <v>1</v>
@@ -7139,7 +7139,7 @@
         <v>0</v>
       </c>
       <c r="Y95" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:25" x14ac:dyDescent="0.25">
@@ -7221,14 +7221,14 @@
     </row>
     <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D97" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
@@ -7352,7 +7352,7 @@
         <v>0</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I99" s="5">
         <v>1</v>
@@ -7403,7 +7403,7 @@
         <v>0</v>
       </c>
       <c r="Y99" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="100" spans="1:25" x14ac:dyDescent="0.25">
@@ -7485,14 +7485,14 @@
     </row>
     <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -7616,7 +7616,7 @@
         <v>0</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I103" s="5">
         <v>1</v>
@@ -7667,7 +7667,7 @@
         <v>0</v>
       </c>
       <c r="Y103" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="104" spans="1:25" x14ac:dyDescent="0.25">
@@ -7749,14 +7749,14 @@
     </row>
     <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D105" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
@@ -7880,7 +7880,7 @@
         <v>0</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I107" s="5">
         <v>1</v>
@@ -7931,7 +7931,7 @@
         <v>0</v>
       </c>
       <c r="Y107" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="108" spans="1:25" x14ac:dyDescent="0.25">
@@ -8013,14 +8013,14 @@
     </row>
     <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B109" s="7"/>
       <c r="C109" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D109" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
@@ -8277,14 +8277,14 @@
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B113" s="7"/>
       <c r="C113" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
@@ -8373,10 +8373,10 @@
         <v>1</v>
       </c>
       <c r="V114" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W114" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X114" s="5">
         <v>0</v>
@@ -8450,10 +8450,10 @@
         <v>1</v>
       </c>
       <c r="V115" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W115" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X115" s="5">
         <v>0</v>
@@ -8527,10 +8527,10 @@
         <v>1</v>
       </c>
       <c r="V116" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W116" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="X116" s="5">
         <v>0</v>
@@ -8541,14 +8541,14 @@
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117" s="7"/>
       <c r="C117" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D117" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="D117" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="V118" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W118" s="2" t="s">
         <v>26</v>
@@ -8714,7 +8714,7 @@
         <v>1</v>
       </c>
       <c r="V119" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W119" s="2" t="s">
         <v>26</v>
@@ -8791,7 +8791,7 @@
         <v>1</v>
       </c>
       <c r="V120" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="W120" s="2" t="s">
         <v>26</v>
@@ -8805,14 +8805,14 @@
     </row>
     <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B121" s="7"/>
       <c r="C121" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D121" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
@@ -8901,10 +8901,10 @@
         <v>1</v>
       </c>
       <c r="V122" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W122" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X122" s="5">
         <v>0</v>
@@ -8978,10 +8978,10 @@
         <v>1</v>
       </c>
       <c r="V123" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W123" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X123" s="5">
         <v>0</v>
@@ -9055,10 +9055,10 @@
         <v>1</v>
       </c>
       <c r="V124" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W124" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="X124" s="5">
         <v>0</v>
@@ -9069,14 +9069,14 @@
     </row>
     <row r="125" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125" s="7"/>
       <c r="C125" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
@@ -9165,7 +9165,7 @@
         <v>1</v>
       </c>
       <c r="V126" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W126" s="2" t="s">
         <v>26</v>
@@ -9242,7 +9242,7 @@
         <v>1</v>
       </c>
       <c r="V127" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W127" s="2" t="s">
         <v>26</v>
@@ -9319,7 +9319,7 @@
         <v>1</v>
       </c>
       <c r="V128" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W128" s="2" t="s">
         <v>26</v>
@@ -9333,14 +9333,14 @@
     </row>
     <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" s="7"/>
       <c r="C129" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D129" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="D129" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="E129" s="7"/>
       <c r="F129" s="7"/>
@@ -9429,10 +9429,10 @@
         <v>1</v>
       </c>
       <c r="V130" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W130" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X130" s="5">
         <v>0</v>
@@ -9506,10 +9506,10 @@
         <v>1</v>
       </c>
       <c r="V131" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W131" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X131" s="5">
         <v>0</v>
@@ -9583,10 +9583,10 @@
         <v>1</v>
       </c>
       <c r="V132" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W132" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X132" s="5">
         <v>0</v>
@@ -9597,14 +9597,14 @@
     </row>
     <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" s="7"/>
       <c r="C133" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D133" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D133" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
@@ -9693,7 +9693,7 @@
         <v>1</v>
       </c>
       <c r="V134" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W134" s="2" t="s">
         <v>26</v>
@@ -9770,7 +9770,7 @@
         <v>1</v>
       </c>
       <c r="V135" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W135" s="2" t="s">
         <v>26</v>
@@ -9847,7 +9847,7 @@
         <v>1</v>
       </c>
       <c r="V136" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W136" s="2" t="s">
         <v>26</v>
@@ -9861,14 +9861,14 @@
     </row>
     <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B137" s="7"/>
       <c r="C137" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
@@ -9957,10 +9957,10 @@
         <v>1</v>
       </c>
       <c r="V138" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W138" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X138" s="5">
         <v>0</v>
@@ -10034,10 +10034,10 @@
         <v>1</v>
       </c>
       <c r="V139" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W139" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X139" s="5">
         <v>0</v>
@@ -10111,10 +10111,10 @@
         <v>1</v>
       </c>
       <c r="V140" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W140" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="X140" s="5">
         <v>0</v>
@@ -10125,14 +10125,14 @@
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B141" s="7"/>
       <c r="C141" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D141" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="E141" s="7"/>
       <c r="F141" s="7"/>
@@ -10221,7 +10221,7 @@
         <v>1</v>
       </c>
       <c r="V142" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W142" s="2" t="s">
         <v>26</v>
@@ -10298,7 +10298,7 @@
         <v>1</v>
       </c>
       <c r="V143" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W143" s="2" t="s">
         <v>26</v>
@@ -10375,7 +10375,7 @@
         <v>1</v>
       </c>
       <c r="V144" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W144" s="2" t="s">
         <v>26</v>
@@ -10389,14 +10389,14 @@
     </row>
     <row r="145" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B145" s="7"/>
       <c r="C145" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E145" s="7"/>
       <c r="F145" s="7"/>

</xml_diff>